<commit_message>
Added various length validations and updated the readme. Still need to update the XSD.
</commit_message>
<xml_diff>
--- a/examples/example8.xlsx
+++ b/examples/example8.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://informatica-my.sharepoint.com/personal/jbowring_informatica_com/Documents/_My Documents/Coding/Windows/Excel/Xml2Xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2021AEB943D295F39B66C2D92063358075101956" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2668A99E-F66A-4463-A125-6818F5D1C495}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_26754DB6434294B9A2895EB4EA2188134BE28837" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BE9B8A00-F994-4911-8417-4A7943A5E014}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Books!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Books!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Title</t>
   </si>
@@ -37,6 +37,15 @@
     <t>Price</t>
   </si>
   <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Addendum</t>
+  </si>
+  <si>
     <t>Everyday Italian</t>
   </si>
   <si>
@@ -47,6 +56,15 @@
   </si>
   <si>
     <t>30.00</t>
+  </si>
+  <si>
+    <t>Some text</t>
+  </si>
+  <si>
+    <t>More text</t>
+  </si>
+  <si>
+    <t>Even more text!</t>
   </si>
   <si>
     <t>Harry Potter</t>
@@ -112,27 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -448,98 +446,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>10</v>
+      <c r="D3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>14</v>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>17</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <dataValidations count="2">
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"FOO,BAR,CAT"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B5" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$B$2:$B$5</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>10</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>10</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>10</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0000-000005000000}">
+      <formula1>10</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" operator="notBetween" allowBlank="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>10</formula1>
+      <formula2>20</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added data validation for values
</commit_message>
<xml_diff>
--- a/examples/example8.xlsx
+++ b/examples/example8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://informatica-my.sharepoint.com/personal/jbowring_informatica_com/Documents/_My Documents/Coding/Windows/Excel/Xml2Xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_26754DB6434294B9A2895EB4EA2188134BE28837" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BE9B8A00-F994-4911-8417-4A7943A5E014}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B9A6FA5-27DA-4514-BC97-257E8CB36C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
@@ -52,12 +52,6 @@
     <t>Giada De Laurentiis</t>
   </si>
   <si>
-    <t>2005</t>
-  </si>
-  <si>
-    <t>30.00</t>
-  </si>
-  <si>
     <t>Some text</t>
   </si>
   <si>
@@ -73,28 +67,16 @@
     <t>J K. Rowling</t>
   </si>
   <si>
-    <t>29.99</t>
-  </si>
-  <si>
     <t>XQuery Kick Start</t>
   </si>
   <si>
     <t>Vaidyanathan Nagarajan</t>
   </si>
   <si>
-    <t>2003</t>
-  </si>
-  <si>
-    <t>49.99</t>
-  </si>
-  <si>
     <t>Learning XML</t>
   </si>
   <si>
     <t>Erik T. Ray</t>
-  </si>
-  <si>
-    <t>39.95</t>
   </si>
 </sst>
 </file>
@@ -130,8 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,18 +433,18 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -493,77 +477,77 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D2" s="2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D3" s="2">
+        <v>29.99</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D4" s="2">
+        <v>49.99</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D5" s="2">
+        <v>39.950000000000003</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <dataValidations count="7">
+  <dataValidations count="10">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"FOO,BAR,CAT"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B5" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$B$2:$B$5</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>10</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>10</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>10</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000004000000}">
@@ -574,6 +558,17 @@
       <formula2>20</formula2>
     </dataValidation>
     <dataValidation type="textLength" operator="notBetween" allowBlank="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>10</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000009000000}">
+      <formula1>10</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="D3" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+      <formula1>10</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="notBetween" allowBlank="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>10</formula1>
       <formula2>20</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Removed the ambiguity of a "value" validation
</commit_message>
<xml_diff>
--- a/examples/example8.xlsx
+++ b/examples/example8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://informatica-my.sharepoint.com/personal/jbowring_informatica_com/Documents/_My Documents/Coding/Windows/Excel/Xml2Xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B9A6FA5-27DA-4514-BC97-257E8CB36C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{881DA607-0118-4C79-B319-1C81948E83C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,10 +478,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>2005</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -501,10 +501,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="1">
-        <v>2005</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2">
-        <v>29.99</v>
+        <v>15.65</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -515,7 +515,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="1">
-        <v>2003</v>
+        <v>-125</v>
       </c>
       <c r="D4" s="2">
         <v>49.99</v>

</xml_diff>